<commit_message>
tabela em uma pagina
</commit_message>
<xml_diff>
--- a/Eventos/Eventos.xlsx
+++ b/Eventos/Eventos.xlsx
@@ -256,85 +256,85 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,179 +694,180 @@
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="10" width="15.875" customWidth="1"/>
+    <col min="3" max="9" width="12.625" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
     <col min="11" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="56.65" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="4" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="56.65" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="62.45" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="62.45" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9">
+      <c r="A4" s="28"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="62.45" customHeight="1" thickBot="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="62.45" customHeight="1" thickBot="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="4">
         <v>4</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="62.45" customHeight="1" thickBot="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="9">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10" ht="62.45" customHeight="1" thickBot="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="15">
         <v>6</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>